<commit_message>
Finishing staging inserts for EI XML
</commit_message>
<xml_diff>
--- a/Spreadsheet/Current Mapping/E I XML Mapping-SP_edits.xlsx
+++ b/Spreadsheet/Current Mapping/E I XML Mapping-SP_edits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\Spreadsheet\Current Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B698F2AE-02B7-4D24-A0E4-B627ADAEDC4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F978D09D-00AA-46BF-8F72-6764EEF813A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="867" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5106,8 +5106,8 @@
   <dimension ref="A1:G228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C212" sqref="C212"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5388,7 +5388,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -5421,12 +5421,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="22"/>
       <c r="C33" s="23"/>
     </row>
-    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>14</v>
       </c>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="C34" s="20"/>
     </row>
-    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>16</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>18</v>
       </c>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="C36" s="20"/>
     </row>
-    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
         <v>20</v>
       </c>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="C37" s="17"/>
     </row>
-    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>21</v>
       </c>
@@ -5473,7 +5473,7 @@
       </c>
       <c r="C38" s="24"/>
     </row>
-    <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>23</v>
       </c>
@@ -10447,7 +10447,7 @@
       </c>
       <c r="C172" s="20"/>
     </row>
-    <row r="173" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="27" t="s">
         <v>20</v>
       </c>
@@ -10456,7 +10456,7 @@
       </c>
       <c r="C173" s="17"/>
     </row>
-    <row r="174" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="18" t="s">
         <v>21</v>
       </c>
@@ -10465,7 +10465,7 @@
       </c>
       <c r="C174" s="24"/>
     </row>
-    <row r="175" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="27" t="s">
         <v>23</v>
       </c>
@@ -10474,19 +10474,19 @@
       </c>
       <c r="C175" s="17"/>
     </row>
-    <row r="176" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B176" s="19"/>
       <c r="C176" s="20"/>
     </row>
-    <row r="177" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="7"/>
       <c r="B177" s="8"/>
       <c r="C177" s="7"/>
     </row>
-    <row r="178" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>243</v>
       </c>
@@ -10494,7 +10494,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>241</v>
       </c>
@@ -15753,7 +15753,7 @@
       </c>
       <c r="C28" s="20"/>
     </row>
-    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>20</v>
       </c>
@@ -19581,12 +19581,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -19594,7 +19594,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -19603,7 +19603,7 @@
       </c>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -19611,7 +19611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -19619,7 +19619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -19628,7 +19628,7 @@
       </c>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -19636,7 +19636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -19644,12 +19644,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -19657,7 +19657,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -20112,7 +20112,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -20123,7 +20123,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -20131,7 +20131,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -20139,7 +20139,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -20148,7 +20148,7 @@
       </c>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -20156,7 +20156,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -20164,12 +20164,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -20177,7 +20177,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Test scripts built an being tested
</commit_message>
<xml_diff>
--- a/Spreadsheet/Current Mapping/E I XML Mapping-SP_edits.xlsx
+++ b/Spreadsheet/Current Mapping/E I XML Mapping-SP_edits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\Spreadsheet\Current Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F978D09D-00AA-46BF-8F72-6764EEF813A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1ED31D-FE66-47DA-AFCF-DDFB7B761938}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="867" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="867" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YTL" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5849" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5848" uniqueCount="752">
   <si>
     <t xml:space="preserve"> id                              </t>
   </si>
@@ -5105,8 +5105,8 @@
   </sheetPr>
   <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
@@ -10819,7 +10819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G226"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B30" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
@@ -11427,9 +11427,7 @@
       <c r="B67" s="16">
         <v>10</v>
       </c>
-      <c r="C67" s="37" t="s">
-        <v>738</v>
-      </c>
+      <c r="C67" s="37"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">

</xml_diff>